<commit_message>
Dataset ready to analyze
</commit_message>
<xml_diff>
--- a/_psychology_project/_data/Base GC Innovación - Cliente.xlsx
+++ b/_psychology_project/_data/Base GC Innovación - Cliente.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haachicanoy/Repositories/Statistical_consulting/_psychology_project/_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B126479A-61FC-6543-9A5D-6E24846F5D0C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="8400" windowHeight="2400"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="25280" windowHeight="14720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base en Codigos" sheetId="1" r:id="rId1"/>
@@ -1061,8 +1067,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1116,11 +1122,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1162,7 +1176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1194,9 +1208,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1228,6 +1260,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1403,16 +1453,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ER52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="EE1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="ER3" sqref="ER3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="148" max="148" width="46.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:148">
+    <row r="1" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1858,7 +1911,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:148">
+    <row r="2" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>58389925</v>
       </c>
@@ -2223,7 +2276,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:148">
+    <row r="3" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>56512040</v>
       </c>
@@ -2525,7 +2578,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:148">
+    <row r="4" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>58181245</v>
       </c>
@@ -2833,7 +2886,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:148">
+    <row r="5" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>58304623</v>
       </c>
@@ -3168,7 +3221,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:148">
+    <row r="6" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>58402271</v>
       </c>
@@ -3506,7 +3559,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:148">
+    <row r="7" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>58023996</v>
       </c>
@@ -3844,7 +3897,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:148">
+    <row r="8" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>57371264</v>
       </c>
@@ -4155,7 +4208,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:148">
+    <row r="9" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>57591397</v>
       </c>
@@ -4481,7 +4534,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:148">
+    <row r="10" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>58066106</v>
       </c>
@@ -4819,7 +4872,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:148">
+    <row r="11" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>56609347</v>
       </c>
@@ -5145,7 +5198,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:148">
+    <row r="12" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>58015222</v>
       </c>
@@ -5444,7 +5497,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:148">
+    <row r="13" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>56739292</v>
       </c>
@@ -5764,7 +5817,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:148">
+    <row r="14" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>57297253</v>
       </c>
@@ -6084,7 +6137,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:148">
+    <row r="15" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>57534327</v>
       </c>
@@ -6392,7 +6445,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:148">
+    <row r="16" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>57413972</v>
       </c>
@@ -6694,7 +6747,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="1:148">
+    <row r="17" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>57543113</v>
       </c>
@@ -6993,7 +7046,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="18" spans="1:148">
+    <row r="18" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>57545186</v>
       </c>
@@ -7283,7 +7336,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="1:148">
+    <row r="19" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>58435790</v>
       </c>
@@ -7606,7 +7659,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:148">
+    <row r="20" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>58403758</v>
       </c>
@@ -7929,7 +7982,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:148">
+    <row r="21" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>57796612</v>
       </c>
@@ -8234,7 +8287,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:148">
+    <row r="22" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>58067514</v>
       </c>
@@ -8584,7 +8637,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="23" spans="1:148">
+    <row r="23" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>57572296</v>
       </c>
@@ -8886,7 +8939,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="1:148">
+    <row r="24" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>57629849</v>
       </c>
@@ -9212,7 +9265,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:148">
+    <row r="25" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>57538980</v>
       </c>
@@ -9541,7 +9594,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:148">
+    <row r="26" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>58302236</v>
       </c>
@@ -9873,7 +9926,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:148">
+    <row r="27" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>58269281</v>
       </c>
@@ -10190,7 +10243,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:148">
+    <row r="28" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>58304251</v>
       </c>
@@ -10492,7 +10545,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="29" spans="1:148">
+    <row r="29" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>56496979</v>
       </c>
@@ -10797,7 +10850,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:148">
+    <row r="30" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>58142058</v>
       </c>
@@ -11099,7 +11152,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:148">
+    <row r="31" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>56501398</v>
       </c>
@@ -11419,7 +11472,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="32" spans="1:148">
+    <row r="32" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>58272214</v>
       </c>
@@ -11736,7 +11789,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:148">
+    <row r="33" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>58268424</v>
       </c>
@@ -12050,7 +12103,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:148">
+    <row r="34" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>58109584</v>
       </c>
@@ -12331,7 +12384,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="35" spans="1:148">
+    <row r="35" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>58133119</v>
       </c>
@@ -12636,7 +12689,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="36" spans="1:148">
+    <row r="36" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>58028102</v>
       </c>
@@ -12959,7 +13012,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="37" spans="1:148">
+    <row r="37" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>58270893</v>
       </c>
@@ -13288,7 +13341,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="38" spans="1:148">
+    <row r="38" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>57615508</v>
       </c>
@@ -13566,7 +13619,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="39" spans="1:148">
+    <row r="39" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>57617439</v>
       </c>
@@ -13913,7 +13966,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="40" spans="1:148">
+    <row r="40" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>58404932</v>
       </c>
@@ -14206,7 +14259,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="41" spans="1:148">
+    <row r="41" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>58354652</v>
       </c>
@@ -14466,7 +14519,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="42" spans="1:148">
+    <row r="42" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>58429420</v>
       </c>
@@ -14726,7 +14779,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="43" spans="1:148">
+    <row r="43" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>58356118</v>
       </c>
@@ -14983,7 +15036,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="44" spans="1:148">
+    <row r="44" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>58357422</v>
       </c>
@@ -15264,7 +15317,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="45" spans="1:148">
+    <row r="45" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>57798310</v>
       </c>
@@ -15566,7 +15619,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="46" spans="1:148">
+    <row r="46" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>58309702</v>
       </c>
@@ -15901,7 +15954,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="47" spans="1:148">
+    <row r="47" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>58308729</v>
       </c>
@@ -16191,7 +16244,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="48" spans="1:148">
+    <row r="48" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>56898950</v>
       </c>
@@ -16493,7 +16546,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="49" spans="1:148">
+    <row r="49" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>58402510</v>
       </c>
@@ -16810,7 +16863,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="50" spans="1:148">
+    <row r="50" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>58268204</v>
       </c>
@@ -17127,7 +17180,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="51" spans="1:148">
+    <row r="51" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>58444211</v>
       </c>
@@ -17414,7 +17467,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="52" spans="1:148">
+    <row r="52" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>57290182</v>
       </c>
@@ -17773,16 +17826,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:ER52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:148">
+    <row r="1" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18228,7 +18281,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:148">
+    <row r="2" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>58389925</v>
       </c>
@@ -18593,7 +18646,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:148">
+    <row r="3" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>56512040</v>
       </c>
@@ -18895,7 +18948,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:148">
+    <row r="4" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>58181245</v>
       </c>
@@ -19203,7 +19256,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:148">
+    <row r="5" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>58304623</v>
       </c>
@@ -19538,7 +19591,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:148">
+    <row r="6" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>58402271</v>
       </c>
@@ -19876,7 +19929,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:148">
+    <row r="7" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>58023996</v>
       </c>
@@ -20214,7 +20267,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:148">
+    <row r="8" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>57371264</v>
       </c>
@@ -20525,7 +20578,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:148">
+    <row r="9" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>57591397</v>
       </c>
@@ -20851,7 +20904,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:148">
+    <row r="10" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>58066106</v>
       </c>
@@ -21189,7 +21242,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:148">
+    <row r="11" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>56609347</v>
       </c>
@@ -21515,7 +21568,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:148">
+    <row r="12" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>58015222</v>
       </c>
@@ -21814,7 +21867,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:148">
+    <row r="13" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>56739292</v>
       </c>
@@ -22134,7 +22187,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:148">
+    <row r="14" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>57297253</v>
       </c>
@@ -22454,7 +22507,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:148">
+    <row r="15" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>57534327</v>
       </c>
@@ -22762,7 +22815,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:148">
+    <row r="16" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>57413972</v>
       </c>
@@ -23064,7 +23117,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="1:148">
+    <row r="17" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>57543113</v>
       </c>
@@ -23363,7 +23416,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="18" spans="1:148">
+    <row r="18" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>57545186</v>
       </c>
@@ -23653,7 +23706,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="1:148">
+    <row r="19" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>58435790</v>
       </c>
@@ -23976,7 +24029,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:148">
+    <row r="20" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>58403758</v>
       </c>
@@ -24299,7 +24352,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:148">
+    <row r="21" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>57796612</v>
       </c>
@@ -24604,7 +24657,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:148">
+    <row r="22" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>58067514</v>
       </c>
@@ -24954,7 +25007,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="23" spans="1:148">
+    <row r="23" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>57572296</v>
       </c>
@@ -25256,7 +25309,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="1:148">
+    <row r="24" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>57629849</v>
       </c>
@@ -25582,7 +25635,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:148">
+    <row r="25" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>57538980</v>
       </c>
@@ -25911,7 +25964,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:148">
+    <row r="26" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>58302236</v>
       </c>
@@ -26243,7 +26296,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:148">
+    <row r="27" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>58269281</v>
       </c>
@@ -26560,7 +26613,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:148">
+    <row r="28" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>58304251</v>
       </c>
@@ -26862,7 +26915,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="29" spans="1:148">
+    <row r="29" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>56496979</v>
       </c>
@@ -27167,7 +27220,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:148">
+    <row r="30" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>58142058</v>
       </c>
@@ -27469,7 +27522,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:148">
+    <row r="31" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>56501398</v>
       </c>
@@ -27789,7 +27842,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="32" spans="1:148">
+    <row r="32" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>58272214</v>
       </c>
@@ -28106,7 +28159,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:148">
+    <row r="33" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>58268424</v>
       </c>
@@ -28420,7 +28473,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:148">
+    <row r="34" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>58109584</v>
       </c>
@@ -28701,7 +28754,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="35" spans="1:148">
+    <row r="35" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>58133119</v>
       </c>
@@ -29006,7 +29059,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="36" spans="1:148">
+    <row r="36" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>58028102</v>
       </c>
@@ -29329,7 +29382,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="37" spans="1:148">
+    <row r="37" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>58270893</v>
       </c>
@@ -29658,7 +29711,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="38" spans="1:148">
+    <row r="38" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>57615508</v>
       </c>
@@ -29936,7 +29989,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="39" spans="1:148">
+    <row r="39" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>57617439</v>
       </c>
@@ -30283,7 +30336,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="40" spans="1:148">
+    <row r="40" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>58404932</v>
       </c>
@@ -30576,7 +30629,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="41" spans="1:148">
+    <row r="41" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>58354652</v>
       </c>
@@ -30836,7 +30889,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="42" spans="1:148">
+    <row r="42" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>58429420</v>
       </c>
@@ -31096,7 +31149,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="43" spans="1:148">
+    <row r="43" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>58356118</v>
       </c>
@@ -31353,7 +31406,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="44" spans="1:148">
+    <row r="44" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>58357422</v>
       </c>
@@ -31634,7 +31687,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="45" spans="1:148">
+    <row r="45" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>57798310</v>
       </c>
@@ -31936,7 +31989,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="46" spans="1:148">
+    <row r="46" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>58309702</v>
       </c>
@@ -32271,7 +32324,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="47" spans="1:148">
+    <row r="47" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>58308729</v>
       </c>
@@ -32561,7 +32614,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="48" spans="1:148">
+    <row r="48" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>56898950</v>
       </c>
@@ -32863,7 +32916,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="49" spans="1:148">
+    <row r="49" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>58402510</v>
       </c>
@@ -33180,7 +33233,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="50" spans="1:148">
+    <row r="50" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>58268204</v>
       </c>
@@ -33497,7 +33550,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="51" spans="1:148">
+    <row r="51" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>58444211</v>
       </c>
@@ -33784,7 +33837,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="52" spans="1:148">
+    <row r="52" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>57290182</v>
       </c>

</xml_diff>